<commit_message>
Add the function 'SH_COL_H' (show/Hide columns, starts hidden) and 'SH_COL_S' (show/Hide columns, starts shown)
</commit_message>
<xml_diff>
--- a/Demos/Etk.Demo.ExcelDna1/Etk.Demo.ExcelDna1.xlsx
+++ b/Demos/Etk.Demo.ExcelDna1/Etk.Demo.ExcelDna1.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Etk\ETK-Git\Demos\Etk.Demo.ExcelDna1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="3330" windowWidth="15360" windowHeight="8040"/>
+    <workbookView xWindow="1380" yWindow="3330" windowWidth="15360" windowHeight="8040" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="7" r:id="rId1"/>
@@ -22,12 +17,12 @@
     <definedName name="DEC_EXEC">#REF!</definedName>
     <definedName name="DEC_STATUS">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725" calcOnSave="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -210,16 +205,22 @@
   </si>
   <si>
     <t>{AmountRoundedToHundred}</t>
+  </si>
+  <si>
+    <t>[SH_COL_H=2::Test_2]</t>
+  </si>
+  <si>
+    <t>[SH_COL_H=1::Test_1]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
   <fonts count="14">
     <font>
@@ -591,19 +592,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -722,14 +723,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -800,6 +801,12 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="10" fillId="18" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -815,6 +822,9 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="10" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -837,6 +847,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="18" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1218,20 +1234,20 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="30.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="30.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="16384" width="30.42578125" style="1"/>
   </cols>
@@ -1241,7 +1257,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -1249,7 +1265,7 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="16384" width="11.42578125" style="1"/>
   </cols>
@@ -1259,15 +1275,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Feuil3"/>
-  <dimension ref="A1:N43"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="52.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="52.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="82.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.28515625" bestFit="1" customWidth="1"/>
@@ -1295,228 +1311,247 @@
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="38"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="2" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="41"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A5" s="2"/>
+      <c r="B5" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="46"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="47"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B6" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="32" t="s">
+      <c r="C6" s="36"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="33"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="B6" s="22" t="s">
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="35"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="B7" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D7" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E7" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F7" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G7" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="30"/>
-      <c r="I6" s="31" t="s">
+      <c r="H7" s="32"/>
+      <c r="I7" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="B7" s="20" t="s">
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="B8" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C8" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D8" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E8" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F8" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N8" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
-    </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="14" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="F10" s="23"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="F11" s="23"/>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H13" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="5"/>
-      <c r="B13" s="15" t="s">
+    <row r="14" spans="1:14">
+      <c r="A14" s="5"/>
+      <c r="B14" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C14" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I14" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
-      <c r="G14" s="5"/>
-      <c r="K14" s="5"/>
-    </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="5" t="s">
+      <c r="G15" s="5"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="5"/>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="5"/>
+      <c r="B17" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C17" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D17" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E17" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F17" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="26" spans="8:10">
-      <c r="J26" s="3" t="s">
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="J27" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="8:10">
-      <c r="H27" s="3" t="s">
+    <row r="28" spans="1:10">
+      <c r="H28" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="I28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J27" s="3" t="s">
+      <c r="J28" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="6:6">
-      <c r="F43" s="26"/>
+    <row r="44" spans="6:6">
+      <c r="F44" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:M6"/>
-    <mergeCell ref="G5:M5"/>
-    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:M7"/>
+    <mergeCell ref="G6:M6"/>
+    <mergeCell ref="B6:F6"/>
     <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1541,7 +1576,7 @@
               <x14:cfIcon iconSet="3ArrowsGray" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>B12</xm:sqref>
+          <xm:sqref>B13</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1550,7 +1585,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Feuil4"/>
   <dimension ref="A1:J11"/>
   <sheetViews>
@@ -1558,7 +1593,7 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.42578125" customWidth="1"/>
     <col min="2" max="2" width="56.28515625" customWidth="1"/>
@@ -1579,10 +1614,10 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="38"/>
+      <c r="C4" s="41"/>
       <c r="D4" s="1" t="s">
         <v>58</v>
       </c>
@@ -1593,15 +1628,15 @@
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="44"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:10">

</xml_diff>